<commit_message>
added leaflet map and initial setup
</commit_message>
<xml_diff>
--- a/data/SiteMetadata.xlsx
+++ b/data/SiteMetadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremiah.blondeau\Documents\R\projects\acropora-monitoring-program\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC43C3CE-496C-49CE-8C54-138D7305F595}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A492BA44-7B4D-4B0D-86BE-7652E9BC14D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27375" windowHeight="16050" xr2:uid="{C2BAA5FA-67E1-48D7-B728-697CD1A55C94}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>Site_Name</t>
   </si>
@@ -61,13 +61,22 @@
   </si>
   <si>
     <t>lon</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>"Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum."</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +91,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -112,6 +127,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,18 +442,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBCF0900-D05D-45C7-99F0-371ED56FC613}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,107 +465,168 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>17.76239</v>
+        <v>17.767130000000002</v>
       </c>
       <c r="C2">
-        <v>-64.587459999999993</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.591610000000003</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3">
-        <v>18.311160000000001</v>
+        <v>18.304659999999998</v>
       </c>
       <c r="C3">
-        <v>-64.837950000000006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.846130000000002</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>18.316800000000001</v>
+        <v>18.317160000000001</v>
       </c>
       <c r="C4">
-        <v>-64.98836</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.988939999999999</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5">
-        <v>17.78556</v>
+        <v>17.762149999999998</v>
       </c>
       <c r="C5">
-        <v>-64.6113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.60087</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>17.785679999999999</v>
+        <v>17.76483</v>
       </c>
       <c r="C6">
-        <v>-64.632180000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.615769999999998</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>18.321860000000001</v>
+        <v>18.31964</v>
       </c>
       <c r="C7">
-        <v>-64.746110000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.743989999999997</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8">
-        <v>18.354240000000001</v>
+        <v>18.356739999999999</v>
       </c>
       <c r="C8">
-        <v>-64.851780000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.854069999999993</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>17.784140000000001</v>
+        <v>17.787009999999999</v>
       </c>
       <c r="C9">
-        <v>-64.750829999999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-64.748670000000004</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B10">
-        <v>18.317219999999999</v>
+        <v>18.315670000000001</v>
       </c>
       <c r="C10">
-        <v>-64.725449999999995</v>
+        <v>-64.726169999999996</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>